<commit_message>
Add new Paylocity Document and Screenshot
</commit_message>
<xml_diff>
--- a/Issues/Paylocity.xlsx
+++ b/Issues/Paylocity.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31473E5A-0F35-4888-8DCC-44A6A864FBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{955D7C13-4A3A-441A-8FFB-BEEFF8716006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,42 +33,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="106">
   <si>
     <t>Test Scenarios</t>
   </si>
   <si>
-    <t xml:space="preserve">Add User </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Login The application </t>
-  </si>
-  <si>
-    <t>2. I am on the Benefits Dashboard page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. Click on Add Employee </t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. I am on the add employee Modal </t>
-  </si>
-  <si>
-    <t>5.-  I should be able to enter employee details</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6. I add First Name as Test </t>
-  </si>
-  <si>
-    <t xml:space="preserve">7. I Add Last Name as Challenge </t>
-  </si>
-  <si>
-    <t xml:space="preserve">8. I add Dependents as 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">9.- Click on Add modal </t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. Verify Columns { Id, LastName, FirstName, Dependents, Salary, Gross,Benefits Cost, Net pay, Actions } showing </t>
+    <t>User Scenario: Add Employee</t>
+  </si>
+  <si>
+    <t>Navigate to the Benefits Dashboard page.</t>
+  </si>
+  <si>
+    <t>Click the "Add Employee" button.</t>
+  </si>
+  <si>
+    <t>The Add Employee modal window opens.</t>
+  </si>
+  <si>
+    <t>Enter the employee details in the form fields:</t>
+  </si>
+  <si>
+    <t>First Name: Enter "Test"</t>
+  </si>
+  <si>
+    <t>Last Name: Enter "Challenge"</t>
+  </si>
+  <si>
+    <t>Dependents: Set the value to "1"</t>
+  </si>
+  <si>
+    <t>Click the "Add" button in the modal.</t>
+  </si>
+  <si>
+    <t>Verify that the following columns appear in the employee table:</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Dependents</t>
+  </si>
+  <si>
+    <t>Salary</t>
+  </si>
+  <si>
+    <t>Gross Pay</t>
+  </si>
+  <si>
+    <t>Benefits Cost</t>
+  </si>
+  <si>
+    <t>Net Pay</t>
+  </si>
+  <si>
+    <t>Actions</t>
   </si>
   <si>
     <t xml:space="preserve">Specification </t>
@@ -274,7 +298,282 @@
     <t>Net salary per paycheck=2000−(38.46+38.46)=2000−76.92=1923.08\text{Net salary per paycheck} = 2000 - (38.46 + 38.46) = 2000 - 76.92 = 1923.08Net salary per paycheck=2000−(38.46+38.46)=2000−76.92=1923.08</t>
   </si>
   <si>
-    <t>Dependents</t>
+    <t>User Scenario: Verify Employee Table Columns</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ensure that the following columns are present in the employee table on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Benefits Dashboard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ID</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Displays the unique identifier for each employee.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>First Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Shows the employee’s first name.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Last Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Shows the employee’s last name.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dependents</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Indicates the number of dependents for each employee.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Salary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Displays the employee's base salary.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Gross Pay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Shows the gross pay before any deductions.</t>
+    </r>
+  </si>
+  <si>
+    <t>Benefits Cost: Displays the cost of the employee’s benefits.</t>
+  </si>
+  <si>
+    <r>
+      <t>Net Pay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Indicates the employee’s pay after deductions for benefits.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Actions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Provides buttons or links for performing actions such as editing or deleting an employee.</t>
+    </r>
+  </si>
+  <si>
+    <t>Scenario 3: Delete Employee</t>
+  </si>
+  <si>
+    <r>
+      <t>GIVEN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I am an employer</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>AND</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I am on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Benefits Dashboard</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> page</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>WHEN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I click the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"Delete"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button under the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Actions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> column for an employee</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>THEN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the selected employee should be removed from the employee list</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Benefit Cost </t>
@@ -441,7 +740,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,8 +770,16 @@
       <name val="Aptos Narrow"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -497,8 +804,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="45">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1056,11 +1381,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1134,18 +1474,23 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1458,6 +1803,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A834EC01-9F4D-4A60-8003-1103E99D313B}" name="Table2" displayName="Table2" ref="A3:A20" totalsRowShown="0">
+  <autoFilter ref="A3:A20" xr:uid="{A834EC01-9F4D-4A60-8003-1103E99D313B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{E90BC3BB-CE18-458D-A7BE-105BC7CF72B8}" name="Navigate to the Benefits Dashboard page."/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5E098240-64DD-4C40-AECA-B6C8E558F3F4}" name="Table1" displayName="Table1" ref="A1:C34" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:C34" xr:uid="{5E098240-64DD-4C40-AECA-B6C8E558F3F4}"/>
   <tableColumns count="3">
@@ -1790,10 +2145,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1806,173 +2161,318 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>9</v>
+      <c r="A12" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>10</v>
+      <c r="A13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>11</v>
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="15.75">
-      <c r="A18" s="2" t="s">
-        <v>13</v>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="15.75">
-      <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="29.25">
-      <c r="A29" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="1" t="s">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15.75">
+      <c r="A33" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="15.75">
-      <c r="A34" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="29.25">
+      <c r="A36" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>26</v>
-      </c>
-    </row>
     <row r="39" spans="1:1">
-      <c r="A39" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="15.75">
+      <c r="A41" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="78"/>
+      <c r="B51" s="78"/>
+      <c r="C51" s="78"/>
+      <c r="D51" s="78"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="78"/>
+      <c r="H51" s="78"/>
+      <c r="I51" s="78"/>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="79" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="80" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="81" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="80" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" s="81" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" s="80" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="80" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="81" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="82" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="83" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="78"/>
+      <c r="B64" s="78"/>
+      <c r="C64" s="78"/>
+      <c r="D64" s="78"/>
+      <c r="E64" s="78"/>
+      <c r="F64" s="78"/>
+      <c r="G64" s="78"/>
+      <c r="H64" s="78"/>
+      <c r="I64" s="78"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="79" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="80" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="80" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="81" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1993,13 +2493,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="15" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="D1" s="4"/>
     </row>
@@ -2495,55 +2995,55 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="19" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E1" s="20" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="F1" s="20" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="G1" s="31" t="s">
-        <v>38</v>
+        <v>61</v>
       </c>
       <c r="H1" s="31" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="I1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="204.75" customHeight="1">
       <c r="A2" s="66" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B2" s="70" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="H2" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="I2" s="41"/>
     </row>
@@ -2554,7 +3054,7 @@
       <c r="D3" s="34"/>
       <c r="E3" s="34"/>
       <c r="F3" s="34" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
@@ -2567,7 +3067,7 @@
       <c r="D4" s="34"/>
       <c r="E4" s="34"/>
       <c r="F4" s="34" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="G4" s="34"/>
       <c r="H4" s="34"/>
@@ -2580,7 +3080,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="G5" s="43"/>
       <c r="H5" s="43"/>
@@ -2599,28 +3099,28 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="67" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B7" s="70" t="s">
-        <v>51</v>
+        <v>74</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D7" s="40" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E7" s="40" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="F7" s="40" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="G7" s="40" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="H7" s="40" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="I7" s="41"/>
     </row>
@@ -2631,7 +3131,7 @@
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
       <c r="F8" s="34" t="s">
-        <v>56</v>
+        <v>79</v>
       </c>
       <c r="G8" s="34"/>
       <c r="H8" s="34"/>
@@ -2644,7 +3144,7 @@
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
       <c r="F9" s="34" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="G9" s="34"/>
       <c r="H9" s="34"/>
@@ -2657,7 +3157,7 @@
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="G10" s="34"/>
       <c r="H10" s="34"/>
@@ -2670,7 +3170,7 @@
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
       <c r="F11" s="43" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="G11" s="43"/>
       <c r="H11" s="43"/>
@@ -2700,22 +3200,22 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="68" t="s">
-        <v>40</v>
+        <v>63</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>60</v>
+        <v>83</v>
       </c>
       <c r="C14" s="51" t="s">
-        <v>42</v>
+        <v>65</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="G14" s="34"/>
       <c r="H14" s="34"/>
@@ -2728,7 +3228,7 @@
       <c r="D15" s="34"/>
       <c r="E15" s="34"/>
       <c r="F15" s="34" t="s">
-        <v>62</v>
+        <v>85</v>
       </c>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
@@ -2741,13 +3241,13 @@
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34" t="s">
-        <v>63</v>
+        <v>86</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="H16" s="34" t="s">
-        <v>65</v>
+        <v>88</v>
       </c>
       <c r="I16" s="42"/>
     </row>
@@ -2805,58 +3305,58 @@
     </row>
     <row r="22" spans="1:9" s="34" customFormat="1">
       <c r="A22" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="B22" s="71" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="B22" s="77" t="s">
+        <v>89</v>
       </c>
       <c r="C22" s="64"/>
       <c r="D22" s="64"/>
       <c r="E22" s="64"/>
       <c r="F22" s="64" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="G22" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="H22" t="s">
-        <v>69</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:9" s="34" customFormat="1">
       <c r="A23" s="61"/>
-      <c r="B23" s="71"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="64"/>
       <c r="D23" s="64"/>
       <c r="E23" s="64"/>
       <c r="F23" s="64" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:9" s="34" customFormat="1">
       <c r="A24" s="61"/>
-      <c r="B24" s="71"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="64"/>
       <c r="D24" s="64"/>
       <c r="E24" s="64"/>
       <c r="F24" s="64" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="34" customFormat="1">
       <c r="A25" s="61"/>
-      <c r="B25" s="71"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="64" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D25" s="64" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="E25" s="64" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="F25" s="64" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="34" customFormat="1">
@@ -2898,9 +3398,9 @@
       <c r="D30" s="64"/>
       <c r="E30" s="64"/>
       <c r="F30" s="64"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="60"/>
@@ -2920,76 +3420,76 @@
       <c r="D32" s="64"/>
       <c r="E32" s="64"/>
       <c r="F32" s="64" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="G32" s="64"/>
-      <c r="H32" s="76"/>
+      <c r="H32" s="34"/>
       <c r="I32" s="42"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="67" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" s="71" t="s">
-        <v>75</v>
+        <v>63</v>
+      </c>
+      <c r="B33" s="77" t="s">
+        <v>98</v>
       </c>
       <c r="C33" s="64"/>
       <c r="D33" s="64"/>
       <c r="E33" s="64"/>
       <c r="F33" s="64" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="G33" s="64"/>
-      <c r="H33" s="76"/>
+      <c r="H33" s="34"/>
       <c r="I33" s="42"/>
     </row>
     <row r="34" spans="1:9" ht="29.25">
       <c r="A34" s="61"/>
-      <c r="B34" s="71"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="64"/>
       <c r="D34" s="64"/>
       <c r="E34" s="64"/>
-      <c r="F34" s="78" t="s">
-        <v>77</v>
+      <c r="F34" s="76" t="s">
+        <v>100</v>
       </c>
       <c r="G34" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="H34" s="76" t="s">
-        <v>79</v>
+        <v>101</v>
+      </c>
+      <c r="H34" s="34" t="s">
+        <v>102</v>
       </c>
       <c r="I34" s="42"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="61"/>
-      <c r="B35" s="71"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="64"/>
       <c r="D35" s="64"/>
       <c r="E35" s="64"/>
       <c r="F35" s="64" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="G35" s="64"/>
-      <c r="H35" s="76"/>
+      <c r="H35" s="34"/>
       <c r="I35" s="42"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="61"/>
-      <c r="B36" s="71"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="64" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D36" s="64" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="E36" s="64" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="F36" s="64" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="G36" s="64"/>
-      <c r="H36" s="76"/>
+      <c r="H36" s="34"/>
       <c r="I36" s="42"/>
     </row>
     <row r="37" spans="1:9">
@@ -3000,7 +3500,7 @@
       <c r="E37" s="64"/>
       <c r="F37" s="64"/>
       <c r="G37" s="64"/>
-      <c r="H37" s="76"/>
+      <c r="H37" s="34"/>
       <c r="I37" s="42"/>
     </row>
     <row r="38" spans="1:9">
@@ -3011,7 +3511,7 @@
       <c r="E38" s="64"/>
       <c r="F38" s="64"/>
       <c r="G38" s="64"/>
-      <c r="H38" s="76"/>
+      <c r="H38" s="34"/>
       <c r="I38" s="42"/>
     </row>
     <row r="39" spans="1:9">
@@ -3022,7 +3522,7 @@
       <c r="E39" s="64"/>
       <c r="F39" s="64"/>
       <c r="G39" s="64"/>
-      <c r="H39" s="76"/>
+      <c r="H39" s="34"/>
       <c r="I39" s="42"/>
     </row>
     <row r="40" spans="1:9">
@@ -3033,19 +3533,19 @@
       <c r="E40" s="64"/>
       <c r="F40" s="64"/>
       <c r="G40" s="64"/>
-      <c r="H40" s="76"/>
+      <c r="H40" s="34"/>
       <c r="I40" s="42"/>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="72"/>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="77"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="75"/>
+      <c r="A41" s="71"/>
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="73"/>
+      <c r="I41" s="74"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="35"/>

</xml_diff>